<commit_message>
Test case1 xcel updated
</commit_message>
<xml_diff>
--- a/data/LoginTest_ID_01.xlsx
+++ b/data/LoginTest_ID_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitbulbu\social-media\TestingFW\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\social_media\TestingExtentReportFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E184AA9-AC36-4A39-9698-C07210E3D9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659FB874-0C81-4A8C-9288-773D683C65D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ayush@19</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>9545351058</t>
+  </si>
+  <si>
+    <t>amruta@12</t>
+  </si>
+  <si>
+    <t>expected_color</t>
+  </si>
+  <si>
+    <t>rgba(56, 88, 152, 1)</t>
   </si>
 </sst>
 </file>
@@ -83,8 +89,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -366,37 +372,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{ED372AFF-371B-4740-9320-B2B3988F243C}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A048D448-C603-49C3-A89E-EF65CCBCA5C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>